<commit_message>
changed mini dataset and corrected some errors
</commit_message>
<xml_diff>
--- a/config/project_files/nbgen.xlsx
+++ b/config/project_files/nbgen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulavaldti-my.sharepoint.com/personal/rodur28_ulaval_ca/Documents/Séquençage/Fcy1_crypto/minidataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2A4DAA-F2C0-4AEC-A2C9-BE1A09883814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{BB3B28A5-B367-41CD-85FC-7F5E33BA5EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E12F0F24-1AF5-4994-979C-E55A7C6E38B1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DC90B287-DF25-4C8B-BFBD-5375494AA6F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Species</t>
   </si>
@@ -56,9 +56,6 @@
     <t>CN</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>T1</t>
   </si>
   <si>
@@ -68,7 +65,13 @@
     <t>r1</t>
   </si>
   <si>
+    <t>r2</t>
+  </si>
+  <si>
     <t>F1</t>
+  </si>
+  <si>
+    <t>alp</t>
   </si>
 </sst>
 </file>
@@ -440,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6CD826-936F-401B-A50A-20D4CD3646D4}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +468,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -476,16 +479,36 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2">
+        <v>5.0432241748072615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2">
-        <v>4.8681064068445554</v>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>5.0433554250353074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added T2 samples to toy dataset
</commit_message>
<xml_diff>
--- a/config/project_files/nbgen.xlsx
+++ b/config/project_files/nbgen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulavaldti-my.sharepoint.com/personal/rodur28_ulaval_ca/Documents/Séquençage/Fcy1_crypto/minidataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulavaldti-my.sharepoint.com/personal/rodur28_ulaval_ca/Documents/gyoza/minidataset/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{BB3B28A5-B367-41CD-85FC-7F5E33BA5EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E12F0F24-1AF5-4994-979C-E55A7C6E38B1}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{BB3B28A5-B367-41CD-85FC-7F5E33BA5EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FF8ECCC-5E1D-488A-A627-9A4E42A48456}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DC90B287-DF25-4C8B-BFBD-5375494AA6F7}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{DC90B287-DF25-4C8B-BFBD-5375494AA6F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Species</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>alp</t>
+  </si>
+  <si>
+    <t>T2</t>
   </si>
 </sst>
 </file>
@@ -443,15 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6CD826-936F-401B-A50A-20D4CD3646D4}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -488,10 +491,10 @@
         <v>6</v>
       </c>
       <c r="F2">
-        <v>5.0432241748072615</v>
+        <v>5.0432241748072597</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -508,7 +511,47 @@
         <v>6</v>
       </c>
       <c r="F3">
-        <v>5.0433554250353074</v>
+        <v>5.0433554250353101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>5.3311498558694383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>5.3617858961319023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>